<commit_message>
Util updated, duplicate names handled
</commit_message>
<xml_diff>
--- a/Doc/Issue list.xlsx
+++ b/Doc/Issue list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="1776" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Description</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>Not Tested</t>
-  </si>
-  <si>
     <t>Backend</t>
   </si>
   <si>
@@ -103,10 +100,7 @@
     <t>Bishal/Navaraj</t>
   </si>
   <si>
-    <t>Fixed in backend</t>
-  </si>
-  <si>
-    <t>Exception handled in backend</t>
+    <t>Tested</t>
   </si>
 </sst>
 </file>
@@ -480,7 +474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,10 +515,16 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -540,6 +540,12 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -554,6 +560,12 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -563,16 +575,16 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -583,16 +595,16 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -603,7 +615,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -612,7 +624,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -623,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -634,7 +646,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -650,6 +668,12 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -659,7 +683,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -668,7 +692,7 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -679,7 +703,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -688,7 +712,7 @@
         <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,6 +721,12 @@
       </c>
       <c r="B13" t="s">
         <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>